<commit_message>
updated fm39 for allocrule 3
</commit_message>
<xml_diff>
--- a/ftest/data/fm49/Min.Max.Ded.Calculation.Example.xlsx
+++ b/ftest/data/fm49/Min.Max.Ded.Calculation.Example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64_2\home\Joh\ktest_new4\ftest\data\fm49\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64\home\Joh\ktest_new\ftest\data\fm49\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6228316B-0B8F-41C7-BF12-882427AD2D79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C36D7FE-E7DC-4C1C-86D0-0F0B8A69857F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{75D5E7CF-EFFD-4508-9A5B-71E86028FB54}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{75D5E7CF-EFFD-4508-9A5B-71E86028FB54}"/>
   </bookViews>
   <sheets>
     <sheet name="MinMaxDed" sheetId="8" r:id="rId1"/>
@@ -34,7 +34,7 @@
     <definedName name="y.over">MinMaxDed!$F$44</definedName>
     <definedName name="y.under">MinMaxDed!$F$43</definedName>
   </definedNames>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -196,36 +196,9 @@
     <t>MinAndMaxDed</t>
   </si>
   <si>
-    <t>Exactly at limit at final level</t>
-  </si>
-  <si>
-    <t>Slightly over limit at final level</t>
-  </si>
-  <si>
-    <t>Slightly under limit at final level</t>
-  </si>
-  <si>
-    <t>All locations well over limit</t>
-  </si>
-  <si>
-    <t>All locations well under limit</t>
-  </si>
-  <si>
-    <t>Under and over limit at max ded level</t>
-  </si>
-  <si>
-    <t>Both under and over limit at min ded level</t>
-  </si>
-  <si>
-    <t>Both over and under limit at min ded level</t>
-  </si>
-  <si>
     <t>Location deductibles and limits, special condition max deductible and policy minimum deductible and limit.</t>
   </si>
   <si>
-    <t>As well as carrying effective deductible through the calculation, we also carry the accumulated amount by which loss has exceeded the limit ("over limit"), and the accumulated amount by which loss is under the limit ("under limit")</t>
-  </si>
-  <si>
     <t>If there are prior level limits and under limit = 0 (contributing losses have all surpassed their limits), then there is no loss adjustment where the delta is less than the amount of over limit</t>
   </si>
   <si>
@@ -250,10 +223,37 @@
     <t>Damage ratios</t>
   </si>
   <si>
-    <t>The following eight scenarios cover the possibilities of over-limit and under-limit where there is first  a max then a min at progressive levels and prior level limits exist.</t>
-  </si>
-  <si>
-    <t>Both under and over limit are carried as +ve amounts. The following logic is only applied when a minimum and/or maximum deductible is present at subsequent levels, leading to a potential loss adjustment</t>
+    <t>4 All locations well over limit</t>
+  </si>
+  <si>
+    <t>5 All locations well under limit</t>
+  </si>
+  <si>
+    <t>6 Both under and over limit at min ded level</t>
+  </si>
+  <si>
+    <t>7 Both over and under limit at min ded level</t>
+  </si>
+  <si>
+    <t>8 Under and over limit at max ded level</t>
+  </si>
+  <si>
+    <t>1 Exactly at limit at min ded level</t>
+  </si>
+  <si>
+    <t>2 Slightly over limit at min ded level</t>
+  </si>
+  <si>
+    <t>3 Slightly under limit at min ded level</t>
+  </si>
+  <si>
+    <t>As well as carrying effective deductible through the calculation, we also carry the accumulated amount by which prior level loss has exceeded the limit ("over limit"), and the accumulated amount by which prior level loss is under the limit ("under limit")</t>
+  </si>
+  <si>
+    <t>Both under and over limit are carried as +ve amounts. The following logic is only applied when a minimum and/or maximum deductible is present at subsequent levels, leading to a potential loss adjustment ("delta")</t>
+  </si>
+  <si>
+    <t>The following eight scenarios cover the possibilities of over-limit and under-limit where there is first  a max then a min at progressive levels and location limits exist.</t>
   </si>
 </sst>
 </file>
@@ -537,39 +537,11 @@
     </xf>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -586,6 +558,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -902,116 +902,115 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9675C8D0-F48E-4A41-AADD-C52642189E6D}">
   <dimension ref="B1:U60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="2" width="54.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="54.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
     <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="14" max="14" width="10.109375" customWidth="1"/>
+    <col min="15" max="15" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:15" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="str">
+    <row r="2" spans="2:15" ht="18" x14ac:dyDescent="0.35">
+      <c r="B2" s="22" t="str">
         <f>"Scenario: "&amp;C11</f>
-        <v>Scenario: All locations well over limit</v>
-      </c>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+        <v>Scenario: 4 All locations well over limit</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C10" s="24"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="M10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C10" s="34"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="M10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="40"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="32"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="K11" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="L11" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="M11" s="37" t="s">
+      <c r="K11" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="L11" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="M11" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="N11" s="37" t="s">
+      <c r="N11" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="O11" s="38" t="s">
+      <c r="O11" s="28" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="K12" s="45"/>
-      <c r="L12" s="43"/>
-      <c r="M12" s="43">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="K12" s="35"/>
+      <c r="L12" s="33"/>
+      <c r="M12" s="33">
         <v>1</v>
       </c>
-      <c r="N12" s="43">
+      <c r="N12" s="33">
         <v>2</v>
       </c>
-      <c r="O12" s="44">
+      <c r="O12" s="34">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>0</v>
       </c>
@@ -1025,23 +1024,23 @@
         <v>3</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="K13" s="41">
+      <c r="K13" s="31">
         <v>1</v>
       </c>
-      <c r="L13" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="M13" s="39">
+      <c r="L13" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="M13" s="29">
         <v>0.2</v>
       </c>
-      <c r="N13" s="39">
+      <c r="N13" s="29">
         <v>0.10050000000000001</v>
       </c>
-      <c r="O13" s="40">
+      <c r="O13" s="30">
         <v>6.7000000000000004E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>1</v>
       </c>
@@ -1055,23 +1054,23 @@
         <v>3000000</v>
       </c>
       <c r="F14" s="4"/>
-      <c r="K14" s="22">
+      <c r="K14" s="21">
         <v>2</v>
       </c>
-      <c r="L14" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="M14" s="39">
+      <c r="L14" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="M14" s="29">
         <v>0.20050000000000001</v>
       </c>
-      <c r="N14" s="39">
+      <c r="N14" s="29">
         <v>0.10075000000000001</v>
       </c>
-      <c r="O14" s="40">
+      <c r="O14" s="30">
         <v>6.7000000000000004E-2</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>5</v>
       </c>
@@ -1088,23 +1087,23 @@
         <v>0.25</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="K15" s="41">
+      <c r="K15" s="31">
         <v>3</v>
       </c>
-      <c r="L15" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="M15" s="39">
+      <c r="L15" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="M15" s="29">
         <v>0.19950000000000001</v>
       </c>
-      <c r="N15" s="39">
+      <c r="N15" s="29">
         <v>0.10050000000000001</v>
       </c>
-      <c r="O15" s="40">
+      <c r="O15" s="30">
         <v>6.7000000000000004E-2</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>2</v>
       </c>
@@ -1118,23 +1117,23 @@
         <v>1000</v>
       </c>
       <c r="F16" s="1"/>
-      <c r="K16" s="22">
+      <c r="K16" s="21">
         <v>4</v>
       </c>
-      <c r="L16" s="39" t="s">
-        <v>31</v>
-      </c>
-      <c r="M16" s="39">
+      <c r="L16" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="M16" s="29">
         <v>0.25</v>
       </c>
-      <c r="N16" s="39">
+      <c r="N16" s="29">
         <v>0.25</v>
       </c>
-      <c r="O16" s="40">
+      <c r="O16" s="30">
         <v>0.25</v>
       </c>
     </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>3</v>
       </c>
@@ -1148,131 +1147,131 @@
         <v>200000</v>
       </c>
       <c r="F17" s="1"/>
-      <c r="K17" s="41">
+      <c r="K17" s="31">
         <v>5</v>
       </c>
-      <c r="L17" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="M17" s="39">
+      <c r="L17" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="M17" s="29">
         <v>0.05</v>
       </c>
-      <c r="N17" s="39">
+      <c r="N17" s="29">
         <v>0.05</v>
       </c>
-      <c r="O17" s="40">
+      <c r="O17" s="30">
         <v>0.05</v>
       </c>
     </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="1"/>
-      <c r="K18" s="22">
+      <c r="K18" s="21">
         <v>6</v>
       </c>
-      <c r="L18" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="M18" s="39">
+      <c r="L18" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="M18" s="29">
         <v>0.05</v>
       </c>
-      <c r="N18" s="39">
+      <c r="N18" s="29">
         <v>0.05</v>
       </c>
-      <c r="O18" s="40">
+      <c r="O18" s="30">
         <v>0.25</v>
       </c>
       <c r="S18" s="16"/>
       <c r="T18" s="16"/>
       <c r="U18" s="16"/>
     </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="24">
+      <c r="C19" s="42">
         <v>1000</v>
       </c>
-      <c r="D19" s="25"/>
+      <c r="D19" s="43"/>
       <c r="E19" s="4"/>
       <c r="F19" s="1"/>
-      <c r="K19" s="41">
+      <c r="K19" s="31">
         <v>7</v>
       </c>
-      <c r="L19" s="39" t="s">
-        <v>35</v>
-      </c>
-      <c r="M19" s="39">
+      <c r="L19" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="M19" s="29">
         <v>0.25</v>
       </c>
-      <c r="N19" s="39">
+      <c r="N19" s="29">
         <v>0.25</v>
       </c>
-      <c r="O19" s="40">
+      <c r="O19" s="30">
         <v>0.05</v>
       </c>
     </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="1"/>
-      <c r="K20" s="42">
+      <c r="K20" s="32">
         <v>8</v>
       </c>
-      <c r="L20" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="M20" s="43">
+      <c r="L20" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="M20" s="33">
         <v>0.25</v>
       </c>
-      <c r="N20" s="43">
+      <c r="N20" s="33">
         <v>0.05</v>
       </c>
-      <c r="O20" s="44">
+      <c r="O20" s="34">
         <v>0.05</v>
       </c>
       <c r="S20" s="16"/>
       <c r="T20" s="16"/>
       <c r="U20" s="16"/>
     </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="24">
+      <c r="C21" s="42">
         <v>5000</v>
       </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="25"/>
+      <c r="D21" s="44"/>
+      <c r="E21" s="43"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="24">
+      <c r="C22" s="42">
         <v>1000000</v>
       </c>
-      <c r="D22" s="26"/>
-      <c r="E22" s="25"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="43"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
         <v>7</v>
       </c>
@@ -1281,7 +1280,7 @@
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:21" x14ac:dyDescent="0.3">
       <c r="C26" s="1">
         <v>1</v>
       </c>
@@ -1295,7 +1294,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>8</v>
       </c>
@@ -1316,7 +1315,7 @@
         <v>1500000</v>
       </c>
     </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>10</v>
       </c>
@@ -1338,7 +1337,7 @@
       </c>
       <c r="H28" s="10"/>
     </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>11</v>
       </c>
@@ -1361,7 +1360,7 @@
       <c r="S29" s="11"/>
       <c r="U29" s="11"/>
     </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B30" s="7" t="s">
         <v>12</v>
       </c>
@@ -1382,7 +1381,7 @@
         <v>600000</v>
       </c>
     </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>15</v>
       </c>
@@ -1403,7 +1402,7 @@
         <v>600000</v>
       </c>
     </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>21</v>
       </c>
@@ -1425,7 +1424,7 @@
       </c>
       <c r="I32" s="10"/>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>20</v>
       </c>
@@ -1447,15 +1446,15 @@
       </c>
       <c r="I33" s="10"/>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B34" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="28">
+      <c r="C34" s="37">
         <f>SUM(C30:D30)</f>
         <v>400000</v>
       </c>
-      <c r="D34" s="28"/>
+      <c r="D34" s="37"/>
       <c r="E34" s="15">
         <f>E30</f>
         <v>200000</v>
@@ -1464,19 +1463,19 @@
         <f>C34</f>
         <v>400000</v>
       </c>
-      <c r="G34" s="30"/>
+      <c r="G34" s="23"/>
       <c r="H34" s="10"/>
       <c r="I34" s="10"/>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="27">
+      <c r="C35" s="36">
         <f>SUM(C32:D32)</f>
         <v>0</v>
       </c>
-      <c r="D35" s="27"/>
+      <c r="D35" s="36"/>
       <c r="E35" s="5">
         <f>E32</f>
         <v>0</v>
@@ -1490,15 +1489,15 @@
       <c r="N35" s="11"/>
       <c r="O35" s="11"/>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B36" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="27">
+      <c r="C36" s="36">
         <f>SUM(C33:D33)</f>
         <v>348000</v>
       </c>
-      <c r="D36" s="27"/>
+      <c r="D36" s="36"/>
       <c r="E36" s="12">
         <v>0</v>
       </c>
@@ -1507,41 +1506,41 @@
         <v>348000</v>
       </c>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B37" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C37" s="29">
+      <c r="C37" s="38">
         <f>SUM(C29:D29)</f>
         <v>2000</v>
       </c>
-      <c r="D37" s="29"/>
+      <c r="D37" s="38"/>
       <c r="E37" s="14"/>
       <c r="F37" s="14"/>
       <c r="G37" s="10"/>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B38" s="21" t="s">
+    <row r="38" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B38" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C38" s="27">
+      <c r="C38" s="36">
         <f>C19</f>
         <v>1000</v>
       </c>
-      <c r="D38" s="27"/>
+      <c r="D38" s="36"/>
       <c r="E38" s="5"/>
       <c r="G38" s="10"/>
       <c r="I38" s="10"/>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B39" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C39" s="28">
+      <c r="C39" s="37">
         <f>MAX(x.loss+MIN(x.effective-deduct3,x.under),0)</f>
         <v>400000</v>
       </c>
-      <c r="D39" s="28"/>
+      <c r="D39" s="37"/>
       <c r="E39" s="8">
         <f>E34</f>
         <v>200000</v>
@@ -1551,21 +1550,21 @@
         <v>600000</v>
       </c>
       <c r="G39" s="16" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="H39" s="10"/>
       <c r="N39" s="16"/>
       <c r="O39" s="16"/>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B40" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C40" s="27">
+      <c r="C40" s="36">
         <f>MAX(x.under-(loss-x.loss),0)</f>
         <v>0</v>
       </c>
-      <c r="D40" s="27"/>
+      <c r="D40" s="36"/>
       <c r="E40" s="5">
         <f>E35</f>
         <v>0</v>
@@ -1576,15 +1575,15 @@
       </c>
       <c r="I40" s="5"/>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>20</v>
       </c>
-      <c r="C41" s="27">
+      <c r="C41" s="36">
         <f>MAX(x.over+(x.loss+x.effective-deduct3)-loss,0)</f>
         <v>349000</v>
       </c>
-      <c r="D41" s="27"/>
+      <c r="D41" s="36"/>
       <c r="E41" s="5">
         <f>E33</f>
         <v>549000</v>
@@ -1595,7 +1594,7 @@
       </c>
       <c r="I41" s="5"/>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>13</v>
       </c>
@@ -1606,10 +1605,10 @@
         <f>F39</f>
         <v>600000</v>
       </c>
-      <c r="G42" s="30"/>
+      <c r="G42" s="23"/>
       <c r="I42" s="10"/>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>21</v>
       </c>
@@ -1624,7 +1623,7 @@
       <c r="N43" s="11"/>
       <c r="O43" s="11"/>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B44" s="11" t="s">
         <v>20</v>
       </c>
@@ -1637,7 +1636,7 @@
       </c>
       <c r="I44" s="10"/>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>23</v>
       </c>
@@ -1654,8 +1653,8 @@
       <c r="N45" s="16"/>
       <c r="O45" s="16"/>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B46" s="21" t="s">
+    <row r="46" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B46" s="45" t="s">
         <v>24</v>
       </c>
       <c r="F46" s="13">
@@ -1669,7 +1668,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B47" s="7" t="s">
         <v>16</v>
       </c>
@@ -1687,10 +1686,10 @@
         <v>597000</v>
       </c>
       <c r="I47" s="16" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B48" s="10" t="s">
         <v>21</v>
       </c>
@@ -1710,7 +1709,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>20</v>
       </c>
@@ -1730,19 +1729,19 @@
         <v>898000</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>14</v>
       </c>
@@ -1763,26 +1762,26 @@
         <v>600000</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C54" s="10"/>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C55" s="10"/>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C56" s="10"/>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C57" s="10"/>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C58" s="10"/>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C59" s="10"/>
       <c r="F59" s="10"/>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C60" s="10"/>
       <c r="F60" s="10"/>
     </row>
@@ -1792,6 +1791,11 @@
     <sortCondition ref="T4:T33"/>
   </sortState>
   <mergeCells count="12">
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C35:D35"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="C41:D41"/>
@@ -1799,11 +1803,6 @@
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C35:D35"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11:E11" xr:uid="{4B63A890-17D6-4214-9736-B90756F63CBA}">

</xml_diff>

<commit_message>
updated for ktools v3.3.5
</commit_message>
<xml_diff>
--- a/ftest/data/fm49/Min.Max.Ded.Calculation.Example.xlsx
+++ b/ftest/data/fm49/Min.Max.Ded.Calculation.Example.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64\home\Joh\ktest_new\ftest\data\fm49\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64\home\Joh\ktest_new2\ftest\data\fm49\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C36D7FE-E7DC-4C1C-86D0-0F0B8A69857F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{815FA661-328C-493F-891F-130C8E2EF6B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{75D5E7CF-EFFD-4508-9A5B-71E86028FB54}"/>
   </bookViews>
   <sheets>
     <sheet name="MinMaxDed" sheetId="8" r:id="rId1"/>
+    <sheet name="expected" sheetId="9" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="deduct2">MinMaxDed!$F$46</definedName>
@@ -34,7 +35,7 @@
     <definedName name="y.over">MinMaxDed!$F$44</definedName>
     <definedName name="y.under">MinMaxDed!$F$43</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,6 +43,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -110,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
   <si>
     <t>Location</t>
   </si>
@@ -254,6 +258,21 @@
   </si>
   <si>
     <t>The following eight scenarios cover the possibilities of over-limit and under-limit where there is first  a max then a min at progressive levels and location limits exist.</t>
+  </si>
+  <si>
+    <t>Total exposure</t>
+  </si>
+  <si>
+    <t>event_id</t>
+  </si>
+  <si>
+    <t>output_id</t>
+  </si>
+  <si>
+    <t>sidx</t>
+  </si>
+  <si>
+    <t>loss</t>
   </si>
 </sst>
 </file>
@@ -493,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -558,15 +577,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -585,7 +596,21 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -902,8 +927,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9675C8D0-F48E-4A41-AADD-C52642189E6D}">
   <dimension ref="B1:U60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -928,7 +953,7 @@
     <row r="2" spans="2:15" ht="18" x14ac:dyDescent="0.35">
       <c r="B2" s="22" t="str">
         <f>"Scenario: "&amp;C11</f>
-        <v>Scenario: 4 All locations well over limit</v>
+        <v>Scenario: Total exposure</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.3">
@@ -973,11 +998,11 @@
       <c r="B11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="40"/>
-      <c r="E11" s="41"/>
+      <c r="C11" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="38"/>
+      <c r="E11" s="39"/>
       <c r="F11" s="16" t="s">
         <v>31</v>
       </c>
@@ -1024,20 +1049,20 @@
         <v>3</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="K13" s="31">
-        <v>1</v>
-      </c>
-      <c r="L13" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="M13" s="29">
-        <v>0.2</v>
-      </c>
-      <c r="N13" s="29">
-        <v>0.10050000000000001</v>
-      </c>
-      <c r="O13" s="30">
-        <v>6.7000000000000004E-2</v>
+      <c r="K13" s="46">
+        <v>-3</v>
+      </c>
+      <c r="L13" t="s">
+        <v>48</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13" s="28">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
@@ -1054,17 +1079,17 @@
         <v>3000000</v>
       </c>
       <c r="F14" s="4"/>
-      <c r="K14" s="21">
-        <v>2</v>
+      <c r="K14" s="31">
+        <v>1</v>
       </c>
       <c r="L14" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M14" s="29">
-        <v>0.20050000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="N14" s="29">
-        <v>0.10075000000000001</v>
+        <v>0.10050000000000001</v>
       </c>
       <c r="O14" s="30">
         <v>6.7000000000000004E-2</v>
@@ -1075,29 +1100,29 @@
         <v>5</v>
       </c>
       <c r="C15" s="6">
-        <f>VLOOKUP($C$11,$L$13:$O$20,2,FALSE)</f>
-        <v>0.25</v>
+        <f>VLOOKUP($C$11,$L$13:$O$21,2,FALSE)</f>
+        <v>1</v>
       </c>
       <c r="D15" s="6">
-        <f>VLOOKUP($C$11,$L$13:$O$20,3,FALSE)</f>
-        <v>0.25</v>
+        <f>VLOOKUP($C$11,$L$13:$O$21,3,FALSE)</f>
+        <v>1</v>
       </c>
       <c r="E15" s="6">
-        <f>VLOOKUP($C$11,$L$13:$O$20,4,FALSE)</f>
-        <v>0.25</v>
+        <f>VLOOKUP($C$11,$L$13:$O$21,4,FALSE)</f>
+        <v>1</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="K15" s="31">
-        <v>3</v>
+      <c r="K15" s="21">
+        <v>2</v>
       </c>
       <c r="L15" s="29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M15" s="29">
-        <v>0.19950000000000001</v>
+        <v>0.20050000000000001</v>
       </c>
       <c r="N15" s="29">
-        <v>0.10050000000000001</v>
+        <v>0.10075000000000001</v>
       </c>
       <c r="O15" s="30">
         <v>6.7000000000000004E-2</v>
@@ -1117,20 +1142,20 @@
         <v>1000</v>
       </c>
       <c r="F16" s="1"/>
-      <c r="K16" s="21">
-        <v>4</v>
+      <c r="K16" s="31">
+        <v>3</v>
       </c>
       <c r="L16" s="29" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="M16" s="29">
-        <v>0.25</v>
+        <v>0.19950000000000001</v>
       </c>
       <c r="N16" s="29">
-        <v>0.25</v>
+        <v>0.10050000000000001</v>
       </c>
       <c r="O16" s="30">
-        <v>0.25</v>
+        <v>6.7000000000000004E-2</v>
       </c>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.3">
@@ -1147,20 +1172,20 @@
         <v>200000</v>
       </c>
       <c r="F17" s="1"/>
-      <c r="K17" s="31">
-        <v>5</v>
+      <c r="K17" s="21">
+        <v>4</v>
       </c>
       <c r="L17" s="29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M17" s="29">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="N17" s="29">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
       <c r="O17" s="30">
-        <v>0.05</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.3">
@@ -1168,11 +1193,11 @@
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="1"/>
-      <c r="K18" s="21">
-        <v>6</v>
+      <c r="K18" s="31">
+        <v>5</v>
       </c>
       <c r="L18" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M18" s="29">
         <v>0.05</v>
@@ -1181,7 +1206,7 @@
         <v>0.05</v>
       </c>
       <c r="O18" s="30">
-        <v>0.25</v>
+        <v>0.05</v>
       </c>
       <c r="S18" s="16"/>
       <c r="T18" s="16"/>
@@ -1191,26 +1216,26 @@
       <c r="B19" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="42">
+      <c r="C19" s="40">
         <v>1000</v>
       </c>
-      <c r="D19" s="43"/>
+      <c r="D19" s="41"/>
       <c r="E19" s="4"/>
       <c r="F19" s="1"/>
-      <c r="K19" s="31">
-        <v>7</v>
+      <c r="K19" s="21">
+        <v>6</v>
       </c>
       <c r="L19" s="29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M19" s="29">
+        <v>0.05</v>
+      </c>
+      <c r="N19" s="29">
+        <v>0.05</v>
+      </c>
+      <c r="O19" s="30">
         <v>0.25</v>
-      </c>
-      <c r="N19" s="29">
-        <v>0.25</v>
-      </c>
-      <c r="O19" s="30">
-        <v>0.05</v>
       </c>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.3">
@@ -1218,19 +1243,19 @@
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="1"/>
-      <c r="K20" s="32">
-        <v>8</v>
-      </c>
-      <c r="L20" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="M20" s="33">
+      <c r="K20" s="31">
+        <v>7</v>
+      </c>
+      <c r="L20" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="M20" s="29">
         <v>0.25</v>
       </c>
-      <c r="N20" s="33">
-        <v>0.05</v>
-      </c>
-      <c r="O20" s="34">
+      <c r="N20" s="29">
+        <v>0.25</v>
+      </c>
+      <c r="O20" s="30">
         <v>0.05</v>
       </c>
       <c r="S20" s="16"/>
@@ -1241,22 +1266,37 @@
       <c r="B21" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="42">
+      <c r="C21" s="40">
         <v>5000</v>
       </c>
-      <c r="D21" s="44"/>
-      <c r="E21" s="43"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="41"/>
       <c r="F21" s="1"/>
+      <c r="K21" s="32">
+        <v>8</v>
+      </c>
+      <c r="L21" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="M21" s="33">
+        <v>0.25</v>
+      </c>
+      <c r="N21" s="33">
+        <v>0.05</v>
+      </c>
+      <c r="O21" s="34">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="42">
+      <c r="C22" s="40">
         <v>1000000</v>
       </c>
-      <c r="D22" s="44"/>
-      <c r="E22" s="43"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="41"/>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.3">
@@ -1300,19 +1340,19 @@
       </c>
       <c r="C27" s="5">
         <f>C14*C15</f>
-        <v>250000</v>
+        <v>1000000</v>
       </c>
       <c r="D27" s="5">
         <f>D14*D15</f>
-        <v>500000</v>
+        <v>2000000</v>
       </c>
       <c r="E27" s="5">
         <f>E14*E15</f>
-        <v>750000</v>
+        <v>3000000</v>
       </c>
       <c r="F27" s="5">
         <f t="shared" ref="F27:F32" si="0">SUM(C27:E27)</f>
-        <v>1500000</v>
+        <v>6000000</v>
       </c>
     </row>
     <row r="28" spans="2:21" x14ac:dyDescent="0.3">
@@ -1321,19 +1361,19 @@
       </c>
       <c r="C28" s="5">
         <f>MAX(C27-C16,0)</f>
-        <v>249000</v>
+        <v>999000</v>
       </c>
       <c r="D28" s="5">
         <f>MAX(D27-D16,0)</f>
-        <v>499000</v>
+        <v>1999000</v>
       </c>
       <c r="E28" s="5">
         <f>MAX(E27-E16,0)</f>
-        <v>749000</v>
+        <v>2999000</v>
       </c>
       <c r="F28" s="5">
         <f t="shared" si="0"/>
-        <v>1497000</v>
+        <v>5997000</v>
       </c>
       <c r="H28" s="10"/>
     </row>
@@ -1430,19 +1470,19 @@
       </c>
       <c r="C33" s="5">
         <f>MAX(C28-C31,0)</f>
-        <v>49000</v>
+        <v>799000</v>
       </c>
       <c r="D33" s="13">
         <f t="shared" ref="D33:E33" si="2">MAX(D28-D31,0)</f>
-        <v>299000</v>
+        <v>1799000</v>
       </c>
       <c r="E33" s="13">
         <f t="shared" si="2"/>
-        <v>549000</v>
+        <v>2799000</v>
       </c>
       <c r="F33" s="14">
         <f t="shared" ref="F33" si="3">SUM(C33:E33)</f>
-        <v>897000</v>
+        <v>5397000</v>
       </c>
       <c r="I33" s="10"/>
     </row>
@@ -1450,11 +1490,11 @@
       <c r="B34" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="37">
+      <c r="C34" s="44">
         <f>SUM(C30:D30)</f>
         <v>400000</v>
       </c>
-      <c r="D34" s="37"/>
+      <c r="D34" s="44"/>
       <c r="E34" s="15">
         <f>E30</f>
         <v>200000</v>
@@ -1471,11 +1511,11 @@
       <c r="B35" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="36">
+      <c r="C35" s="43">
         <f>SUM(C32:D32)</f>
         <v>0</v>
       </c>
-      <c r="D35" s="36"/>
+      <c r="D35" s="43"/>
       <c r="E35" s="5">
         <f>E32</f>
         <v>0</v>
@@ -1493,41 +1533,41 @@
       <c r="B36" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="36">
+      <c r="C36" s="43">
         <f>SUM(C33:D33)</f>
-        <v>348000</v>
-      </c>
-      <c r="D36" s="36"/>
+        <v>2598000</v>
+      </c>
+      <c r="D36" s="43"/>
       <c r="E36" s="12">
         <v>0</v>
       </c>
       <c r="F36" s="12">
         <f>C36</f>
-        <v>348000</v>
+        <v>2598000</v>
       </c>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B37" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C37" s="38">
+      <c r="C37" s="45">
         <f>SUM(C29:D29)</f>
         <v>2000</v>
       </c>
-      <c r="D37" s="38"/>
+      <c r="D37" s="45"/>
       <c r="E37" s="14"/>
       <c r="F37" s="14"/>
       <c r="G37" s="10"/>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B38" s="45" t="s">
+      <c r="B38" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="C38" s="36">
+      <c r="C38" s="43">
         <f>C19</f>
         <v>1000</v>
       </c>
-      <c r="D38" s="36"/>
+      <c r="D38" s="43"/>
       <c r="E38" s="5"/>
       <c r="G38" s="10"/>
       <c r="I38" s="10"/>
@@ -1536,11 +1576,11 @@
       <c r="B39" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C39" s="37">
+      <c r="C39" s="44">
         <f>MAX(x.loss+MIN(x.effective-deduct3,x.under),0)</f>
         <v>400000</v>
       </c>
-      <c r="D39" s="37"/>
+      <c r="D39" s="44"/>
       <c r="E39" s="8">
         <f>E34</f>
         <v>200000</v>
@@ -1560,11 +1600,11 @@
       <c r="B40" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C40" s="36">
+      <c r="C40" s="43">
         <f>MAX(x.under-(loss-x.loss),0)</f>
         <v>0</v>
       </c>
-      <c r="D40" s="36"/>
+      <c r="D40" s="43"/>
       <c r="E40" s="5">
         <f>E35</f>
         <v>0</v>
@@ -1579,18 +1619,18 @@
       <c r="B41" t="s">
         <v>20</v>
       </c>
-      <c r="C41" s="36">
+      <c r="C41" s="43">
         <f>MAX(x.over+(x.loss+x.effective-deduct3)-loss,0)</f>
-        <v>349000</v>
-      </c>
-      <c r="D41" s="36"/>
+        <v>2599000</v>
+      </c>
+      <c r="D41" s="43"/>
       <c r="E41" s="5">
         <f>E33</f>
-        <v>549000</v>
+        <v>2799000</v>
       </c>
       <c r="F41" s="10">
         <f>SUM(C41:E41)</f>
-        <v>898000</v>
+        <v>5398000</v>
       </c>
       <c r="I41" s="5"/>
     </row>
@@ -1632,7 +1672,7 @@
       <c r="E44" s="12"/>
       <c r="F44" s="12">
         <f>F41</f>
-        <v>898000</v>
+        <v>5398000</v>
       </c>
       <c r="I44" s="10"/>
     </row>
@@ -1654,7 +1694,7 @@
       <c r="O45" s="16"/>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B46" s="45" t="s">
+      <c r="B46" s="36" t="s">
         <v>24</v>
       </c>
       <c r="F46" s="13">
@@ -1673,7 +1713,7 @@
         <v>16</v>
       </c>
       <c r="C47" s="5"/>
-      <c r="F47" s="15">
+      <c r="F47" s="47">
         <f>IF(y.under=0,uloss,oloss)</f>
         <v>600000</v>
       </c>
@@ -1718,15 +1758,15 @@
       <c r="E49" s="5"/>
       <c r="F49" s="14">
         <f>IF(y.over&gt;0,l.over,H49)</f>
-        <v>895000</v>
+        <v>5395000</v>
       </c>
       <c r="G49" s="20">
         <f>MAX(y.over+(y.loss+y.effective-deduct2)-uloss,0)</f>
-        <v>895000</v>
+        <v>5395000</v>
       </c>
       <c r="H49" s="20">
         <f>MAX(y.over+(y.loss+y.effective-deduct2)-H47,0)</f>
-        <v>898000</v>
+        <v>5398000</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.3">
@@ -1786,16 +1826,11 @@
       <c r="F60" s="10"/>
     </row>
   </sheetData>
-  <sortState ref="R4:U33">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R4:U33">
     <sortCondition ref="S4:S33"/>
     <sortCondition ref="T4:T33"/>
   </sortState>
   <mergeCells count="12">
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C35:D35"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="C34:D34"/>
     <mergeCell ref="C41:D41"/>
@@ -1803,14 +1838,188 @@
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C35:D35"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11:E11" xr:uid="{4B63A890-17D6-4214-9736-B90756F63CBA}">
-      <formula1>$L$13:$L$20</formula1>
+      <formula1>$L$13:$L$21</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DFB1B79-9FC3-4CE9-8E73-84D3F9774E9E}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>-3</v>
+      </c>
+      <c r="D2">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>-1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>597000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>598000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>596500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>295000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>346000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>546000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11">
+        <v>446000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>